<commit_message>
basic stats and visualization
</commit_message>
<xml_diff>
--- a/interim/global_embassies_stats.xlsx
+++ b/interim/global_embassies_stats.xlsx
@@ -951,7 +951,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>['fr', 'en', 'ar', 'nl', 'undetected']</t>
+          <t>['so', 'fr', 'en', 'nl', 'undetected']</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -976,7 +976,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>['tr', 'fr', 'mk', 'en', 'id', 'ar', 'hr']</t>
+          <t>['tr', 'fr', 'sl', 'mk', 'en', 'id', 'ar', 'hr']</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>['pt', 'nl', 'fr', 'de', 'uk', 'en', 'es', 'it', 'ar', 'undetected', 'ca']</t>
+          <t>['pt', 'nl', 'fr', 'de', 'uk', 'en', 'es', 'it', 'id', 'ar', 'undetected', 'ca']</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>['so', 'hu', 'es', 'en', 'ar']</t>
+          <t>['es', 'ar', 'en', 'hu']</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">

</xml_diff>

<commit_message>
added language and hashtag data and visualization
</commit_message>
<xml_diff>
--- a/interim/global_embassies_stats.xlsx
+++ b/interim/global_embassies_stats.xlsx
@@ -941,22 +941,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>['nl', 'sv', 'en']</t>
+          <t>['en' 'nl' 'sv']</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>['ar', 'es', 'en']</t>
+          <t>['es' 'en' 'ar']</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>['so', 'fr', 'en', 'nl', 'undetected']</t>
+          <t>['fr' 'en' 'nl' 'undetected' 'ar']</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>['ar', 'fa']</t>
+          <t>['ar' 'fa']</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -966,67 +966,68 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['so', 'de', 'hu', 'en', 'es', 'id', 'ar', 'undetected', 'ca']</t>
+          <t>['es' 'undetected' 'en' 'so' 'ca' 'de' 'hu' 'ar' 'id']</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>['da', 'en']</t>
+          <t>['en' 'da']</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>['tr', 'fr', 'sl', 'mk', 'en', 'id', 'ar', 'hr']</t>
+          <t>['en' 'mk' 'ar' 'hr' 'fr' 'tr' 'id']</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>['ar', 'en', 'so', 'fr']</t>
+          <t>['ar' 'so' 'en' 'fr']</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>['so', 'cy', 'en', 'ar', 'undetected']</t>
+          <t>['en' 'ar' 'undetected' 'so' 'cy']</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>['af', 'ar', 'en', 'undetected']</t>
+          <t>['en' 'ar' 'undetected' 'af']</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>['es', 'undetected']</t>
+          <t>['undetected' 'es']</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>['pt', 'nl', 'fr', 'de', 'uk', 'en', 'es', 'it', 'id', 'ar', 'undetected', 'ca']</t>
+          <t>['fr' 'pt' 'en' 'ar' 'undetected' 'nl' 'es' 'de' 'uk' 'ca' 'it' 'sw']</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>['pt', 'so', 'cy', 'de', 'ro', 'hu', 'es', 'en', 'it', 'id', 'ar', 'vi', 'undetected', 'ca']</t>
+          <t>['es' 'en' 'undetected' 'ca' 'pt' 'so' 'id' 'de' 'it' 'vi' 'cy' 'ar' 'hu'
+ 'sw']</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>['ar', 'en', 'fr']</t>
+          <t>['en' 'fr' 'ar']</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>['en', 'undetected']</t>
+          <t>['undetected' 'en']</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>['es', 'ar', 'en', 'hu']</t>
+          <t>['ar' 'en' 'es' 'hu']</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>['fr', 'pl', 'en', 'id', 'ar']</t>
+          <t>['en' 'pl' 'id' 'fr' 'ar']</t>
         </is>
       </c>
     </row>
@@ -1038,92 +1039,227 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>['#QatarSustainabilityWeek', '#EuropeanDayofLanguages', '#EU-#GCC', '#QatarNationalDay2022', '#GBV', '#COP27', '#WorldCup', '#NEDQAT', '#SDG', '#QSW2022', '#NothingLikeOranje', '#OrangeTheWorld', '#HumanRightsWeek', '#JointCommittees', '#NEDUSA', '#climate', '#molqtr', '#MilitaryAI:', '#NLAgainstGBV', '#HumanRightsDay', '#WaterAction.', '#HumanRightsWeek.', '#Sustainability', '#NEDARG', '#16Days,', '#ForNature', '#SENNED', '#Qatar!', '#WomenHumanRightsDefendersDay.', '#oliebol', '#UNDay,', '#NLagainstGBV', '#NEDECU', '#worldcup2022', '#16Days', '#WK2022', '#UN2023WaterConference', '#Netherlands', '#WorldCup2022']</t>
+          <t>['Register' "Let's" '🇳🇱' nan 'Today' 'Hi' 'QUARTER-FINAL' 'Thanks' '📢'
+ 'Great' 'Oranje' 'As' 'The' 'It’s' 'HE' 'Minister' 'Are' 'Tonight,'
+ 'Gender-based' 'Millions' 'Match' 'A' 'Het' 'Building' 'During' 'We'
+ 'Today’s' 'On' 'Sustainability']</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>['#DocumentaciónEspañola', '#DiaDelCineEspañol', '#Qatar2022', '#DíaDeLaConstitución', '#FelizAñoNuevo.', '#RegistroConsular', '#Qatar', '#Doha', '#España,', '#مشيرب', '#CopaMundialFIFA', '#ElMomentoDeNuestroCine', '#LaListaDeTodos!', '#VamosEspaña', '#ConstituciónEspañola', '#FIFAWorldCup,', '#Qatar.', '#منصة_مشيرب', '#قطر', '#MOIQatar', '#12deOctubre', '#TuConsulado', '#feliz2023', '#Catar2022', '#Qatar,', '#6D', '#QatarNationalDay,', '#España', '#12deoctubre', '#votorogado.', '#12O', '#QatarNationalLibrary.', '#DiaDeLaFiestaNacional', '#CelebramosEspaña']</t>
+          <t>['Desde' nan 'Coincidiendo' 'Hoy' 'Conditions' 'SM' '📲' 'El' '✍️🏻' 'La'
+ 'Si' '🔸"هنا' 'Visitors' 'Celebración' 'Con' '#DiaDelCineEspañol'
+ '📽️Celebramos' 'Ya']</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>['#StandUp4HumanRights', '#NoDeathPenalty', '#BehindTheScenes', '#TeamEurope', '#BELEGY', '#StandWithUkraine', '#UNGA', '#WorldCup', '#قطر،', '#Doha', '#employment.', '#multilateralism:', '#qatarsustainabilityweek', '#SDG8', '#OrangeTheWorld', '#SelectedbyPwC', '#FIFAWorldCup', '#كتارا', '#WISH2022', '#UNDay', '#qsw2022', '#Sinterklaas', '#UNDay!', '#FIFAWorldCup,', '#Qatar.', '#DEVILTIME', '#KingsDay,', '#MOIQatar', '#OneLove', '#Israel', '#MerciEden', '#HealingTheFuture', '#endGBV', '#recap', '#SDGPavilion', '#Belgium', '#MultilateralismMatters', '#بلجيكا', '#DEVILTIME!', '#EU', '#Qatar,', '#Lebanon', '#16Days', '#WorldcupQatar2022', '#Qatar’s', '#AbolitionNow', '#MOFAQatar', '#Belgiuma', '#SDGs.', '#SaintNicolas', '#consular', '#Katara,']</t>
+          <t>['Je' nan 'Today' '📣' 'Sadly' 'All' 'A' 'December' 'Brimming' 'Our' '🧡'
+ '🇶🇦' 'Foreign' 'Deputy' 'De' '⚽️' '#DEVILTIME' 'Team' "It's" 'Derniers'
+ '11,59' '🚨Just' 'To' '👑' '#qatarsustainabilityweek' 'Belgium' 'The'
+ 'Maj.' 'Getting' '❌' 'Yesterday' 'Opening' 'سعادة' 'Luhansk,']</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>['#ایران', '#Qatar2022', '#كأس_العالم_2022', '#FIFAWorldCup', '#كأس_العالم', '#جام_جهانی', '#مونديال', '#هیاکارت', '#تا_پای_جان_برای_ایران', '#قطر', '#مونديال_قطر_2022', '#تا_پای_جان_برای_ایران✌️', '#جام_جهانی✌️', '#Iran', '#دوحة', '#ھیا', '#المنتخب_الايراني', '#تیم_ملی', '#جام_جهانی_2022', '#WorldcupQatar2022', '#الیوم_الوطني_القطری', '#تیم_ملی_قهرمان', '#كأس_العالم_قطر_2022']</t>
+          <t>[nan 'تتقدم' 'در' 'نظر' '🔻پیام' 'رهبر' 'گوشه' '«شکوه' 'شکوه' 'و' '⚽️'
+ 'این' 'حضور' '#تا_پای_جان_برای_ایران' 'هواداران' '🔴' 'دارندگان'
+ '♦️اطلاعیه/' '🔻آنچه' 'پیرو' 'وصول' 'کاروان' 'ساعاتی' 'تحدث' 'گفتگوی' 'به']</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[nan]</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['#Norteamérica2026.', '#CMQ22', '#CentroMéxicoQatar2022🇲🇽', '#PublicDiplomacyMX', '#Qatar2022', '#EducaciónParaTodasyTodos', '#Mexico', '#NorteAmérica2026,', '#PolíticaExteriorFeminista', '#DiplomaciaPúblicaMX', '#VolandoJuntasyJuntosConDoctorasConAlas', '#OrgulloMexicano', '#ComunicadoSRE', '#Mx', '#Qatar2022🇶🇦,', '#MiConsulado.', '#MéxicoEnQatar', '#كتارا', '#Qonexion', '#Altar', '#Rusia2018,', '#TrophyTour', '#Qatar22', '#Qatar2022,', '#كتارا_ملتقى_الثقافات', '#Cooperación', '#CentroMéxicoQatar2022.', '#VotoExtranjero', '#HechoDeLosMexicanos', '#Norteamérica2026🇲🇽🇺🇸🇨🇦.', '#ElDespertador', '#orangeday', '#Ohtli', '#LatinAmerica', '#Qatar2022…', '#Qatar2022⚽️?', '#VDS', '#TalentoMX', '#Qatar🇶🇦:', '#PublicDiplomacy', '#MásOportunidades', '#mexicoargentina', '#Qatar2022?🇶🇦', '#Mexico’s', '#BarahatAlJanoub', '#QNA', '#EducaciónADistancia', '#Multiversity', '#MéxicoDeMiVida!', '#AltarDeMuertos', '#mundial', '#Qatar2022!', '#consular', '#الشبكة_الدبلوماسية_العامة_العالمية', '#ProtecciónConsular', '#GuiaDelViajero', '#DoctorasConAlas', '#CercaDeTi', '#EducationCity', '#VDS⚕️', '#BelievingIsMagic', '#NosVemosEn2026', '#Sudáfrica2010🇿🇦', '#CMQ.', '#Qatar2022🇶🇦🏆,', '#Argentina', '#SeeYouIn2026', '#ColoresOloresSabores', '#Qatat2022.', '#DiaDeMuertos!', '#DayOfTheDead', '#MexicoVsArabia', '#Bienvenidas', '#InternationalPoliceCooperationCenter', '#CentroMéxicoQatar.', '#MéxicoDeMiVida💚🤍♥️', '#RosarioCastellanos,', '#Qatar🇶🇦,', '#Qatar2022⚽️,', '#DíaNaranja,', '#Latinoamérica.', '#Qatar🇶🇦y', '#ProtecciónConsular.', '#DiplomaciaDeportivaMX', '#CopaFIFA2022⚽️Como', '#Mexico,', '#MEX', '#Norteamérica2026', '#DiaDeMuertos,', '#WebcamsMX', '#qatarnationalday2022', '#كتارا،', '#DiadeMuertos2022', '#JuntosLoHacemosBien🇲🇽🤝🇶🇦', '#CentoMéxicoQatar2022', '#Qatar2022.⚽', '#Qatar2022⚽️🇶🇦', '#LaMagiaDeCreer', '#EstrategiaYDiplomaciaPública', '#DiplomaciaPública🇲🇽🤝🇶🇦.1/2', '#Caribbean,', '#CentroMéxicoQatar2022?', '#DEAPQatar', '#كاسالعالمقطر_2022', '#México86🇲🇽se', '#CentroMéxicoQatar,', '#974', '#DoctorasMexicanasPorElMundo', '#MarruecosvsFrancia?', '#CopaFIFA2022', '#ProtecciónConsular🇲🇽#CentroMexicoQatar2022', '#QatarWorldCup2022?', '#Qatar2022⚽️.', '#Lusail.', '#México.', '#Rusia2018🇷🇺', '#GaleríaM7', '#México', '#TMEC', '#JapónCorea2002', '#OrgulloSEM', '#Norteamérica2026🇲🇽🇺🇸🇨🇦⚽️y', '#MexicoVsArabia?', '#CMQ2022', '#MexVsPol', '#TalentoMexicano', '#GuíaDelViajero', '#Qatar', '#Doha', '#FIFAWorldCup!', '#قطر،', '#Qatar2022🇶🇦!', '#GraziaDeledda.', '#Qatar2022🇶🇦.', '#OrangeTheWorld', '#MéxicoDeMiVida🫶🏻', '#FIFAWorldCup', '#centroméxicoqatar2022', '#ProtecciónPreventiva', '#Monterrey', '#Argentina78!', '#Qatar2022?🇶🇦⚽️', '#EquidadDeGénero', '#Norteamérica2026🇲🇽🇺🇸🇨🇦', '#𝐃𝐨𝐡𝐚', '#Qatar2022...', '#CentroMexicoQatar', '#Qatar2022"', '#Qatar2022?', '#ÁnguloLatino', '#المكسيك', '#EducaciónIME', '#Qatar.', '#CielitoLindo', '#قطر', '#talentomexicano', '#LosMexiquenses', '#EspaciosPúblicosMéxico', '#MexiHouse', '#Doha🇶🇦', '#كأسالعالم', '#Qatar!', '#HayyaCard.', '#educaciónsuperior', '#SIRME?', '#اليوم_الوطني_القطري', '#الوعد2022', '#PrepaEnLineaSEP', '#CentroMéxicoQatar', '#Qatar,', '#ArabianAdventures.', '#SIRME.', '#MEXPOL', '#Qatar?', '#Futbol', '#MX', '#CentroMexicoQatar2022', '#DiplomaciaPúblicaMx', '#GPDNET', '#Brasil2014🇧🇷', '#DatoMundialista', '#MéxicoDeMiVida', '#Qatar202', '#Iztapalapa', '#CentroMéxicoQatar2022', '#WebcamsMx', '#QatarWorldCup2022', '#EnVIVO', '#DíaDeMuertos', '#ViveMiSeleccion', '#Doha,', '#ColoresAromasySabores', '#DiaMundialdelaLuchaContraelCancerdeMama', '#MéxicoVsArabia?', '#SIRME', '#جريدة_الراية', '#FILAH2022', '#Lusailstadium', '#MexvsPol', '#MujerMexicanaMigrante', '#BuenasPrácticas.', '#FIFAWorldCupQatar2022', '#QatarNationalDay', '#Querétaro', '#CentroMéxicoQatar2022,', '#Amistad', '#Literatura.', '#Qatar2022🇶🇦🎉', '#somosunsoloequipo', '#IPCC.', '#DiaDeMuertos', '#EnVivo', '#Mex', '#MundialQatar2022', '#MiConsulado', '#الشبكة_الدبلوماسية_العامة_العالمية،', '#المركز_المكسيكي_القطري2022', '#FMFporNuestroFútbol', '#HayyaCard', '#Qatar2022⚽️!', '#GRULAC', '#Qatar2022.', '#Katara.', '#México70🇲🇽', '#Guadalajara', '#VRME', '#DiaDeLosMuertos', '#CopaDelMundo2022', '#CentroMexicoQatar20222', '#مكسيكوسيتي', '#FIFA', '#Katara,']</t>
+          <t>['3/3' nan '#EstrategiaYDiplomaciaPública' '#MásOportunidades' '¿Sabías'
+ '@LEGORRETA_ARQS' '¡Gran' 'Después' 'El' 'Leaving' 'التهاني' 'En' '🏆' 'A'
+ '"Mi🇲🇽querido' 'Vas' '🧵1/3' 'Recibimos' 'Un' 'Nos' '▶️' 'Agradecemos'
+ 'La' 'Con' 'Conoce' '📌Si' '📢A' '📸' '#CentroMexicoQatar2022' 'Agradecimos'
+ 'Afición' '𝑼𝒏𝒂' '📌¡Si' '¿Estás' 'Cerca' 'Espléndida' '📢' 'Mexican'
+ 'Mexicanos/as' '✍️' '#ComunicadoSRE' '📝' '#Qatar2022' '🎙️@ALFZEGBE:'
+ 'Atención' 'Este' 'Estrategia' 'Horas' '🇲🇽🗣️' 'Que' '32' 'Charro'
+ '@Tralexita1' '¡Gracias' '¡Hoy' '¡Entusiasta' '📌' '⚠️Nuestra' 'Despite'
+ '▶️Si' '⚽️✴️La' 'Guillermo' 'Damos' '1/2' 'Para' '@RafaelLaveagaR'
+ 'Debutamos' '🚨Invitamos' 'Actualización-los' 'Terminando'
+ '.@miseleccionmx' '🤩¡Con' 'Estás' 'Compartiendo' 'Si' '1/3' '🇲🇽¡𝐀𝐪𝐮𝐢́'
+ 'Empezando' 'سعادة' '¡Un' 'Desde' 'Seguimos' 'Colegas' '🇦🇷🇲🇽' '¿Por'
+ 'Recuerda' 'Y' 'Toma' '✅' '¡Bienvenido' 'Muy' '¡Enhorabuena!' 'H.E'
+ 'كلمة' '🚨' '@AnguloNTN24' '¡Evita' '2/2🚨' '🎉' '@miseleccionmx'
+ 'PodcastIMR🎙️' 'Had' '¡Se' '▶️¿Vienes' '¡#LeleMundialista' '📢Atención'
+ '❗️Si' '@DiplomaciaPubl' '➡️' '🗣️¡Estamos' '¡Los' 'Hoy' 'Sofia' 'De'
+ '#CentroMéxicoQatar2022' '¡En' '@FIFAWorldCup' 'Coming' '¡Comienza'
+ '¡Felicidades!' '¡Felicidades' '🎉Entusiasta' 'Aquí' 'Es' 'Welcome'
+ '¡Estamos' '🧵Muchas' 'México' '¡Así' '¡Faltan' 'Su' '▶️¡Faltan' 'Mi'
+ 'Los' '#EnVivo' 'Inicia' '💀🕯️' '🧵A' '¡Aquí' 'Ofrecí' '¡La' 'Asistí' '📣'
+ 'Importantes' '🇲🇽▶️' 'Estamos' 'Anunciamos' '🔶' 'Gracias,'
+ '#DatoMundialista' '“La' '¡Falta' 'Buenos' 'On' '#Mexico' '#SeeYouIn2026'
+ '🇲🇽Si' 'Mexico,' '#MiConsulado' 'Mural' 'تدشين' '🔴سعادة' 'يسرّنا'
+ 'Special' 'We' '💀🌻' 'من' '📣Join' '¿Vienes' 'Yon' '⚠️Si' '▶️¡Estamos'
+ '🔵"Volemos' '🇲🇽🟣' 'Fue' 'Las' '🇲🇽⚽️Aficionadx' '📄' '🇲🇽' '¿Vendrás'
+ '⚽️¡Ya' 'Platicamos' '🇲🇽¿Vienes' '🗣️Faltan' '#EnVIVO' '🥳Del' 'Mexicanx'
+ '¿🇲🇽Vives' '¿Eres' 'Me' '"في' '¡No' '🇲🇽Mexicanx' '🇲🇽✈️🇶🇦¿Vienes' '⌛️']</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>['#Denmark', '#YES', '#FV22', '#equality', '#UNDay', '#leadership', '#security', '#DenmarkInTheUAE', '#DK4UNSC', '#IRENA', '#peace']</t>
+          <t>['Very' 'HE' 'I' nan 'Yesterday' '#UNDay' '⚠️']</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>['#Serbian', '#MadenOcağıPatlama', '#NationalDay', '#UNMIK', '#Оrlovi', '#Qatar2022', '#MDULS', '#video👇', '#GenderEquality,', '#HumanRightsDay2022', '#OrrangeTheWorld', '#WorldCup', '#volleyball', '#Serbia,', '#Qatar', '#UNSC', "#Turkiye's", '#madenpatlama', '#16DaysOfActivism', '#NewYork', '#TeamSerbia', '#قطر2022', "#Bartın'da", '#FIFAWorldCup', '#GenderBasedViolence', '#Türkiye', '#Женева', '#Bartin', '#КФОР', '#orlovi', '#UN', '#AtlasLions', '#FSS', '#16DaysOfActivism.', '#MinaKaradžić', '#Selakovic:', '#CoalMineExplosion', '#LetsOrangeTheWorld', '#FIFAWorldCupQatar2022', '#QatarNationalDay', '#SrcemSvim', '#Srbija', '#Vienna,', '#Serbia', '#Shura_Council,', '#MediaFreedom', '#Изјава', '#ПетарПрви,', '#OrangeTheWorld,', '#تلفزيون_قطر', '#WWCH2022', '#Дачић.', '#FIFAWorldCup.', '#SafetyOfJournalists,', '#Selakovic', '#Kosovo', '#Селаковић', '#Amasra', '#Србија', '#Metohija.', '#Orlovi', '#Dacic', '#FIFAWorldCup🇶🇦', '#QNA', '#GECF', '#Срби', '#WorldCupQatar2022', '#ArmisticeDay,', '#WorldCup2022', '#SoJ2022', '#LestWeForget', '#Austria']</t>
+          <t>[nan 'Последњи' 'FIFA' 'Happy' 'Embassy' 'Président' '🧡' 'Амбасада'
+ 'Главу' 'НЕ' '🇷🇸' 'Talking' 'أهم' 'Statement' 'The' 'Group' 'On' 'Данас'
+ 'During' '#WorldCupQatar2022' 'Charge' 'Visitors' 'У' 'Many' 'شهد' 'In'
+ 'One' '©️🇷🇸' '#Изјава' 'FM' '#Serbia' "#Bartın'da" 'Shocked' 'Sun'
+ 'Министар']</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>['#الشرق', '#قطر2022', '#FIFAWorldCup', '#المونديال_شرقي', '#Qatar2022', '#Morocco', '#المغرب_بلجيكا', '#AtlasLions', '#أسود_الأطلس', '#كاس_العالم_قطر_2022', '#FIFAWorldCupQatar2022', '#DimaMaghrib']</t>
+          <t>[nan '#المونديال_شرقي' '📌']</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>['#TheRedWall', '#FIFAWorldCup2022.', '#iamsomebody', '#Qatar2022', '#FootballforPeace', '#England', '#Welsh', '#ENGSEN', '#كتارا', '#تحدّ_العنف_لاتغض_الطرف', '#UKinQatar', '#كتارا_ملتقى_الثقافات', '#DefeatDaesh,', '#FIFAWorldCup2022', '#Iran', '#BlackHistoryMonth', '#الدوحة', '#WorldCup,', '#BritsinKSA', '#LionsDen', '#DayOfTheGirl', '#SeeThingsDifferently.', '#QNA', '#USAvWAL', '#ArBenYByd', '#Wales.', '#تشارلز_الثالث', '#TogetherStronger', '#WorldCupQatar2022', '#قطر.', '#StreetChildWorldCup', '#BeOnTheBall', '#بريطانيا', '#WorldCup', '#UK', '#كأس_العالم_2022', '#TîmCymru', '#كوكبك_عنوانك', '#Katara', '#ArmisticeDay', '#لأجل_الناجين_ومع_الناجين', '#France', '#Reshuffle', '#ThreeLions', '#تايفون', '#WALUSA', '#WorldCup2022', '#LestWeForget', '#Qatar🇶🇦', '#QNA_Infographic', '#hayya', '#GREATCreativity.', '#Qatar', '#Doha', '#قطر،', '#العلاقات_البريطانية_القطرية🇬🇧🇶🇦', '#لوّن_العالم_بُرتقاليًا', '#FIFAWorldCup', '#المملكة_المتحدة', '#ukinqatar', '#Qatar2022™.', '#ENGLAND', '#RedWall', '#SheLeads', '#YWalGoch', '#WeScoredFirst', '#اليوم_العالمي_للفتاة', '#قطر', '#seethingsdifferently', '#وحدتنا_مصدر_قوتنا', '#GreatCreativity', '#FIFAWorldCup.', '#UKinqatar', '#SeeThingsDifferently', '#worldmentalhealthday', '#GREATCreativity', '#العنف_الجنسي', '#اليوم_الوطني_القطري', '#IDPWD', '#TravelAware', '#كأس_العالم_2022⚽️', '#الوعد2022', '#Qatar,', '#ريشي_سوناك', '#IDG2022', '#EntenteCordiale', '#WorldcupQatar2022', '#InsideAIR', '#England.', '#تشارلز_الثالث.', '#USMNT', '#EnglandvsUSA', '#travelaware', '#WorldCup2022,', '#QatarWorldCup2022', '#RedArrows', '#FIFAWorldcup', '#Iamsomebody', '#WALENG', '#Senegal', '#USA', '#IDG', '#إنهاء_العنف_الجنسي_في_حالات_النزاع', '#FIFAWorldCupQatar2022', '#FIFAWorldCup,', '#TeamCymru', '#Wales', '#ENGvsWales', '#ItsComingHome?', '#العلاقات_البريطانية_القطرية', '#SCWC', '#Qatar2022.', '#CmonCymru', '#OurEngland', '#كأس_العالم_قطر_2022', '#لندن', '#Katara,']</t>
+          <t>[nan 'A' '⚽' 'The' 'خالص' 'What' 'Who' 'With' 'This' 'Enjoyed'
+ '#GreatCreativity' 'Building' '#QNA_Infographic' 'While' 'Huge' 'Our'
+ 'England' 'Busy' 'Come' 'Good' 'Are'
+ '🏴\U000e0067\U000e0062\U000e0065\U000e006e\U000e0067\U000e007f' 'Thank'
+ 'Meet' 'Citizens' 'Is' 'Congratulations' 'Hats' 'Today' 'Interested'
+ 'Ahead' 'Of' 'رئيس' 'As' 'So' 'Ambassador' 'Before' 'PM,' '🧵' 'One'
+ '🇸🇦Saudi' 'Traveling' 'You' "You'll" 'Just' 'It’s' 'Was' "That's" 'أمسية'
+ 'Matchday' 'To' 'من' 'If' 'Highlights' 'اليوم' 'Don’t' 'إن' 'يواجه'
+ 'المباراة' 'صور' 'From' 'كجزء' 'Well' 'سعدت' 'Pleased' 'Great' 'Pob'
+ '🇺🇸🏴\U000e0067\U000e0062\U000e0077\U000e006c\U000e0073\U000e007f' 'Best'
+ 'Fe' 'Do' 'Some' 'بعد' 'المنتخب' '#LestWeForget' "It's" 'كلمة' 'For'
+ 'Less' 'Residents' 'Wondering' 'WATCH:' 'ظلّ' 'جلالة' 'After' 'UK' 'كم'
+ 'هؤلاء' 'These' 'سعادة' 'My' '#StreetChildWorldCup' 'Planning' 'It'
+ 'الشعار']</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>['#TwoMoreSleeps', '#UNGA77', '#TBT:', '#NoDeathPenalty', '#القطرية', '#TastesLikeAustralia', '#Qatar2022', '#COP27', '#QatarWorldCup2022', '#GiveIt100', '#WeAreMatildas', '#roundof16!', '#RemembranceDay', '#meetourspeakers', '#AusCOP27', '#Qatar', '#الأسترالية', '#Denmark!', "#Qatar's", '#قطر2022', '#FIFAWorldCup', '#JointCommittees', '#Australia', '#GoAustralia', '#UNDay', '#Aussie!', '#Socceroos?', '#Socceroos', '#Qatar.', '#HomeAwayFromHome', '#NZ', '#قطر', '#Qatar:', '#Our_Unity_Is_Our_Strength', '#giveit100', '#الخارجية_القطرية', '#وحدتنا_مصدر_قوتنا', '#HappyVegemite', '#auspol', '#France', '#MECGA', '#Qatar_National_Day', '#أستراليا', '#GoSocceroos', '#اليوم_الوطني_القطري', '#VeteransDay', '#socceroos', '#FIFAWWC', '#Qatar,', '#Tunisia!', '#Qatari', '#Australia!', '#Qatar2022.', '#Tunisia.', '#WorldcupQatar2022', '#GiveIt100!', '#AllForSocceroos', '#Australian', '#MOFAQatar', '#beyondgreatness', '#webinar', '#BeyondGreatness', '#engineering_making_life_happen', '#Argentina,', '#LestWeForget']</t>
+          <t>[nan 'Our' 'Next' 'Outstanding' 'Congratulations' 'لقد' 'The' 'Thanks'
+ 'Just' '#TBT:' 'And' 'If' 'As' 'It’s' 'So' 'Australia' '#Aussie!' 'Let’s'
+ 'I' 'من' 'Wishing' 'Thank' 'أمسية' 'A' 'Go' 'Assistant' 'It' 'Australian'
+ 'Was' 'We’re' '1️⃣' 'OPEN' 'Who' '🎧Tune' '#FIFAWorldCup' 'For' 'Register'
+ 'Welcome' 'Today' 'What' 'يسر' 'مساعد' "Can't" 'From' 'Coming' 'On'
+ 'History' 'Pleased' 'EAQC' 'Only' 'Qatar' "I'll" '"The' 'Further' 'Are'
+ 'Great' '#Qatar:' 'Looking']</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[nan]</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>['#المغرب_فرنسا', '#SamiraDjouadi', '#الدوحة.', '#servicepublic', '#ساحة_الأعلام.', '#FIFAWorldCup2022.', '#MIAPark', '#FiersDetreBleus', '#Qatar2022', '#droitshumains,', '#إنجلترا_فرنسا', '#Ukrainian', '#QataNews', '#LusailMuseum.', '#UNGA', '#CoupeDuMondeFIFA', '#CampusFrance,', '#كتارا', '#FRATUN', '#QNA_Sports', '#المغرب', '#Givenchy', '#قطر2022.', '#ENGFRA', '#FIFAWorldCupQatar!', '#Qatar2022,', '#DELF', '#Doha.', '#journey', '#ArtMillMuseum2030.', '#LePetitPrince.', '#كتارا_ملتقى_الثقافات', '#قطر٢٠٢٢', '#FIFAWorldCup2022', '#أوكسير', '#GuinessWordRecord', '#Argentina.', '#ماكرون:', '#لبنان', '#SabriLamouchi', '#library', '#سورية', '#TUNFRA', '#Yeebhom', '#GivenchyBeauty', '#lepetitprince', '#GardezLaCoupeALaMaison', '#الأعوام_الثقافية', '#متاحف_قطر', '#SAFAR', '#تلال_كتارا،', '#الدوحة', '#Argentina_France', '#Qatar_2022', '#QNA', '#FIFAWorldCup|', '#Russia', '#ميثاق_الأمم_المتحدة', '#VOGTLandscapeArchitects.', '#هل_تعلم', '#فرنسا،', '#WorldcupQatar2022.', '#WorldCupQatar2022', '#الفرانكوفونية', '#قطر.', '#Bleus.', '#فرنسا_المغرب', '#للزرق', '#Fiersdetrebleus', '#إيمانويل_ماكرون', '#doha', '#PetitPrince', '#française', '#LePetitPrince', '#موجمبا', '#QNA_Video', '#بيت_التلة', '#قطر_ميناسا_2022', '#WorldCup', '#frenchfootball', '#الأفغان', '#كأس_العالم_FIFA', '#الزرق', '#مجلس_قناة_الكاس', '#DOHA.', '#كأس_العالم_2022', '#franceinfo', '#كأس_العالم', '#SonjaPark', '#sportàvie,', '#قطر!', '#France.', '#استاد_البيت', '#الأمير_الصغير.', '#كاس_العالم_قطر_2022', '#LesBleus', '#TheLittlePrince.', '#Charte', '#الأرجنتين', '#France', '#World_Cup', '#AlThumamaStadium', '#ArtMillMuseum', '#قنا_رياضي', '#ICSC', '#ballondor', '#أيام_الجاليات', '#QatarNews', '#AllezLesBleus', '#SeeYouInQatar', '#FRA', '#BallonDor', '#GoldenBall', '#EU', '#قنوات_الكاس', '#نيويورك', '#جيرو', '#ThreeLions', '#CDM2022.Un', '#أفغانستان.', '#ساحة_الأعلام', '#مرسال_قطر', '#NobelPrize', '#CoupeDuMonde', '#francemaroc', '#KB9', '#WorldCup2022', '#الأمير_الصغير', '#بغداد', '#NY,', '#ArtMillMuseum,', '#Lusail.', '#المجلس', '#FRQA50', '#Qatar🇶🇦', '#CDM2022', '#BLEUS', '#باريس،', '#CommunityDays', '#sportavie', '#SamiraDjouadi,', '#COP27', '#فرنسا_قطر50', '#سوق_واقف', '#فرنسا_بولندا', '#VOGTLandscapeArchitects', '#francophonie', '#نهائي_كاس_العالم_الارجنتين_فرنسا', '#Qatar', '#Doha', '#M7.👏', '#قطر،', '#المغرب؟', '#لوسيل.', '#Liban', '#باريس.', '#قطر2022', '#filmscreenings', '#FIFAWorldCup', '#thelittleprince', '#إنجلترا', '#العنابي', '#FIFAWorldCupQatar.', '#Guinguette,', '#نهائي_كأس_العالم', '#ARGFRA', '#كأس_العالم_2022_قطر', '#لوسيل', '#Qatar.', '#قطر', '#HerzogdeMeuron', '#consulaire', '#Annabi', '#FIFAWorldCup.', '#قطر_2022', '#solarpower', '#ساحة_الاعلام', '#SolidaritéUkraine', '#Total,', '#أستراليا', '#Auxerre', '#𝐁𝐚𝐥𝐥𝐨𝐧𝐝𝐎𝐫', '#Qatar!', '#كأس_العالم_قطر_2022.', '#France,', '#AllezlesBleus', '#Bleus,', '#qatar', '#Qatar_France', '#Bleus!', '#BallondOr', '#FASEJ', '#الأرجنتين_فرنسا', '#الوعد2022', '#باريس', '#غاليري_لافاييت_الدوحة.', '#MOFAQatar', '#KierunekKatar', '#bestplayer', '#ILoveQatar', '#français', '#نديب_قطر', '#Ukraine', '#Bleus', '#QATAR2022', '#مجلس_قنوات_الكاس', '#فرنسا:', '#France_Qatar_2020', '#JourneedesNationsUnies', '#فرنسا_الدنمارك', '#RitzParis', '#QNA_Sport', '#StandWithUkraine', '#العالم_العربي', '#ANGFRA', '#أكاديمية_أسباير', '#FRAAUS', '#QatarWorldCup2022', '#Allez_les_bleus', '#ديما_مغرب', '#FRAANG', '#كاس_العالم_FIFA', '#التنوّع_البيولوجي', '#الزرق.', '#Doha,', '#FiersdetreBleus', '#Lusail', '#Audiences', '#كأس_العالم_قطر2022', '#Bagdad,', '#FlagPlaza,', '#بالفيديو', '#allezlesbleus', '#FlagPlaza', '#FRADAN', '#FIFAWorldCupQatar2022', '#Louvre', '#مونديال_قطر_2022', '#فرنسا_قطر_2020', '#FRAPOL', '#الخارجية_القطرية', '#UNDay2022', '#Majomba', '#FRAMAR', '#Paris2024', '#franceinoman', '#المونديال_مع_الجزار', '#coupedumonde2022', '#الوطن_الرياضي', '#femmes,', '#unBateaupourlUkraine', '#Afghans,', '#فرنسا', '#العربية،', '#Gardezlacoupealamaison', '#Elemental', '#france', '#POL', '#عالوعد', '#Qatar2022.', '#FIFAWorldCupQatar2022.', '#BREAKING', '#Afghanistan,', '#كأس_العالم_قطر_2022', '#beINFWC2022', '#education']</t>
+          <t>[nan 'France🇫🇷' 'La' '#العالم_العربي' '#Qatar' 'بمناسبة'
+ '#التنوّع_البيولوجي' 'Votre' 'Les' 'Bravo' 'Nous' 'شكرا' 'MERCI' '💔' 'Au'
+ 'Allez,' '𝘼𝙇𝙇𝙀𝙕' 'C’est' 'مباراة' 'Match' 'Voici' 'حماس' '𝙳𝚎𝚛𝚗𝚒𝚎̀𝚛𝚎𝚜'
+ '🇦🇷🇫🇷' '#بالفيديو' 'Et' 'Un' '"On' 'French' '4️⃣' '💌' '#مجلس_قناة_الكاس'
+ 'An' '🎥|' '🗣' '🔴' '𝟮𝗲' '🏆' 'الرئيس' 'مبابي' 'Direction' '𝐎𝐍' 'Merci'
+ 'Encore' 'Coup' 'Quelle' 'انطلاق' 'Joie' 'توقعاتكم' 'Plus' 'هل' '🇫🇷🇶🇦|'
+ '#QNA_Video' 'Prêts' 'Deschamps' 'Une' '🫡' 'Tomorrow,' 'Demain'
+ '#Audiences' 'وزيرة' '🧨💥' 'Bonjour' 'الحضور' 'Notre' 'ديشامب' 'EN' 'Mais'
+ '⏸️' 'Cette' 'ALLEZ' 'May' 'À' '𝗘𝗡𝗦𝗘𝗠𝗕𝗟𝗘' 'Échange' 'Arrivée'
+ '@equipedefrance' '🇨🇵أو' 'Place' '🔜' 'كرم' 'مبروك' '💬' "C'est" 'السفير'
+ 'الف' 'هدف' 'Grand' 'Fact!!!' '⚽️' '𝑆𝑒𝑢𝑙' '𝗢𝗡' '𝐔𝐧𝐞' 'GIMS,' 'أمسية'
+ 'شكرًا' 'جزيل' 'Remerciements' 'Très' 'Ce' 'Après' '𝘾𝙝𝙖𝙦𝙪𝙚' "📍C'est"
+ 'Toujours' 'سافرا' 'Ils' '𝙌𝙐𝘼𝙇𝙄𝙁𝙄𝙀𝙎' '𝙆𝙔𝙇𝙄𝘼𝘼𝘼𝘼𝘼𝘼𝘼𝘼𝙉' 'QNA' '𝘾𝙤𝙪𝙥'
+ 'المشجعون' 'عودة' 'زيارة' 'Déplacement' 'Retour' '🤝' '📸|' 'L’ambiance'
+ '𝙋𝙧𝙚𝙢𝙞𝙚̀𝙧𝙚' "71'" 'Kyliaaaaaaaan' 'OLIVIER' 'Réaction' "L'ambassade"
+ 'Belle' '𝐿𝑒' '𝗛𝗮̂𝘁𝗲' '#Qatar2022' 'حفل' 'Cérémonie' 'وزير' 'The'
+ 'Heureux' 'لحظة' 'سعيد' 'After' 'Moment' 'Conférence' '1er' '👏The'
+ 'لقطات' 'بعد' '#BREAKING' 'وصل' 'الجماهير' 'عاجل:' 'Bienvenue' '📸' '👋'
+ '#Paris2024' 'اللقاء' 'Le' 'Fier' 'اختتاماً' 'مساعد' 'Vous' 'قائمة' '𝙇𝙖'
+ 'Afin' 'تُعقد' '⏳' 'استضافة' 'تشرّفت' 'جان' '#سورية' 'Dans' 'Son' 'أود'
+ '#Ukraine' '🇪🇺' 'Two' 'سعادة' '#FRQA50' 'أسعدتني' 'مقر' 'Ravi' 'To'
+ 'Visite' 'سُعدت' 'شاركت' '"بغداد' '22' '«' 'احتفلنا' 'Célébration'
+ 'Plaisir' '"متحف' 'معرض' '"سفر"' 'يكشف' 'L’expo.' 'Ukraine' '28/08/2024'
+ 'H.E' '🎥' 'Striker' '🇶🇦' 'HH' 'لقاء' 'سعدني' 'I' 'Karim' 'KARIM'
+ 'Delighted' 'Mission' 'احتفت' "L'invitée" '#UNGA' '@QatarTelevision'
+ 'أسعدني' '🇶🇦📖❤️The' 'تَمّ' 'أشكر' '@Qatar_Museums' 'En' '#lepetitprince'
+ 'Je' 'قراءة' '@LettheWorldread' '56' 'L’exposition' "☀️Aujourd'hui,"
+ 'بالإنابة' 'زُوروا' 'أتقدّم' 'شرّفني' 'Venez' 'A' 'BREAKING' 'تعرفوا'
+ 'بحضور' 'سيريل' 'يوري' '1/2)' "L'exposition" 'Sur' 'On' 'يلتقي'
+ 'Sustainability']</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>['#Qatar2022', '#البرازيل', '#England', '#QTerminals', '#HRV', '#مونديال_قطر', '#Messi.', '#VamosArgentina', '#Tango', '#argentina', '#SantaCruz', '#tango', '#ExportacionesRecord', '#Messi', '#TrophyTour', '#️⃣1️⃣0️⃣', '#QNA_Sports', '#Milonga', '#Qatar2022,', '#Doha.', '#FinDelMundo', '#ElAviónDeLaSelección', '#MOIQatar', '#36DaysToGo', '#Neuquén,', '#MALVINAS', '#Polonia', '#TodosJuntos!', '#الأرجنتين_بولندا', '#powerful', '#Ushuaia', '#LaRutaNatural', '#MundialQatar2022.', '#Our_Unity_Source_of_Our_Strength', '#mexicoargentina', '#dynamic', '#Doha!', '#QNA', '#dance', '#milonga', '#SEN', '#mundial', '#ENG', '#Qatar2022!', '#ArgentinaTeBusca', '#EducationCity', '#Croacia', '#Argentina', '#Arruabarrena.', '#RíoNegro,', '#WorldCup', '#UK', '#AUS', '#NuevaFotoDePerfil', '#Antártida', '#كأس_العالم', '#Katara', '#exciting', '#Abuelas45años', '#World_Cup_2022', '#كاس_العالم_قطر_2022', '#إيطاليا', '#ARG,', '#الأرجنتين', '#SportsDiplomacy', '#ElSentimientoDeUnPaís', '#FIFAFanFestival', '#MEX', '#Malvinas', '#GolDelAgro', '#afq', '#NaturalezaAlFin', '#VamosArgentina.', '#قنا_رياضي', '#TélamEnQatar', '#كأس_العالم_FIFA_قطر2022', '#ليونيل_ميسي', '#SeleccionArgentina', '#FRA', '#FRA,', '#CelesteyBlanco', '#قنوات_الكاس', '#TodosJuntos', '#afaqatar', '#BuenFinde', '#DíaDeLaONU🇦🇷🇺🇳', '#LaScaloneta?', '#KSA,', '#قنا_إنفوجرافيك', '#Maradona', '#Reconocimiento', '#BoletínDeNoticias', '#ExtraBerries', '#ElMesDel10', '#BRA', '#TeamDioin', '#مونديال_قطر2022', '#México', '#LUSAIL', '#nochedehinchas', '#Patagonia', '#Qatar', '#Doha', '#MalvinasNosUne', '#CopaMundialFIFA', '#قطر2022', '#FIFAWorldCup', '#DiplosEnAcción', '#Katara,', '#profesionalismo', '#Australia', '#إنجلترا', '#CataratasDay', '#WISHQatar2022', '#DigitalDiplomacy', '#NED', '#Qatar2022?', '#Qatar.', '#Chubut,', '#Qatar2022💫', '#قطر', '#مارادونا', '#RankingFIFA', '#46DaysToGo', '#FIFAWorldCup.', '#vocaciondeservicio', '#BuenosAires', '#DiplosEnAccion', '#Qatar!', '#FIFAWolrdCup', '#Corniche.', '#ديبالا', '#ARGMEX', '#Qatar,', '#entertainment', '#nowisall', '#BornBrave', '#Argentina,', '#Mexico86', '#WorldcupQatar2022', '#FIFAWorldCupQatar2022,', '#WorldCup2002', '#SelecciónMayor', '#NowIsAll', '#16días', '#Argentina!', '#QATAR2022', '#QNA_Sport', '#CentroMéxicoQatar2022', '#Mundial', '#QatarWorldCup2022', '#CopaMundial', '#Doha,', '#AspireSummit22', '#CreeEnTuContinente', '#USA', '#41DaysToGo', '#LaAlbiceleste,', '#FIFARanking', '#mallofqatar', '#Malevo', '#FIFAWorldCupQatar2022', '#LaScaloneta', '#ARGENTINA!', '#Argentiniandancegroup', '#TierradelFuego,', '#TodosJuntos...', '#PaísesBajos', '#DiploAr', '#ARG', '#Qatar_National_Day', '#Doha:', '#TierraDelFuego', '#Roadto2022', '#VisitArgentina', '#argentinafansqatar', '#SaludMental', '#drumming', '#POL', '#DeportesRED92', '#Qatar2022.', '#DiegoEterno', '#LaScaloneta.', '#Argentinaa', '#CopaMundialFIFA.', '#MEX.', '#كأس_العالم_قطر_2022', '#carneargentina', '#FIFA', '#AContramano:', '#POR', '#QATAR']</t>
+          <t>['Chau' nan 'Qatar' '🍒🇦🇷🇶🇦' 'Argentina' 'Faro' '¡Se' '@Guille__Nicolas'
+ 'Despedimos' 'Al' 'Los' '🇦🇷' 'Lionel' 'Muchas' '#Qatar2022'
+ '#NuevaFotoDePerfil' '¡PÓNGANLE' 'Lifting' '@Argentina' 'ADD' '¡NO'
+ 'OPERATIVO' '#Our_Unity_Source_of_Our_Strength' '¡Hoy' 'HAPPY' '⚽' '¡Que'
+ 'Con' "Couldn't" 'ℹ️' '📢' '¡¡@Argentina' '🍒' 'Thank' '“Muchaaaachos”'
+ '💙🤍💙' '🇶🇦🇦🇷' 'CELEBRACION' 'Alojamiento' 'It' '#TodosJuntos' '¡#ARG' '¡'
+ '¡Así' 'La' 'El' '¡El' 'The' '🇦🇷🇦🇺' 'Conditions' 'Sí,' '¡Ya'
+ 'Clasificados' '“Muchaaaaaachos”' '🚈' 'أهازيج' 'Nuestro' 'Bueno,'
+ '¡VAMOS' 'Publicamos' 'Guillermo' '¡𝐅𝐈𝐄𝐒𝐓𝐀' '¡Muchas' 'Así' 'Bienvenido'
+ '📸' 'OFICIAL' '¡Gracias' '¡Ganó' '¡Momento' '@ordorica_g' '¡¡¡VAMOS'
+ 'الجماهير' 'Your' 'En' 'Participamos' 'DÍA' '✈️' 'Witness' 'Tras'
+ 'Estamos' '¿Manijas' '🇶🇦' 'Podés' '🤔' '🚌' '🏬' '🇦🇷🇲🇽' '#FIFAWorldCup'
+ '¡Llegó' '¡Acá' 'Durante' 'High' 'GALA' 'Faltan' 'Get' 'Si'
+ '#SelecciónMayor' 'Mi' 'IN' 'Yendo' '📲' '¡Bienvenida' '¡Ahora' '💾'
+ 'Sugerimos' 'IMPORTANTE:' '🏆' '🎶' 'Guía' 'Tickets?' '📱' '🏟️ESTADIO'
+ '@pepeotegui' 'This' '4️⃣' 'Un' '¿Dijeron' '¡La' 'Chants' 'Nuestros'
+ '#قنا_إنفوجرافيك' 'Ya' 'Este' 'Bienvenidos' 'Después' '¡Qatar' 'WATCH'
+ 'سعادة' 'Hoy' 'Ubicado' 'Celebramos' '#Malvinas' 'FIESTA' '👆🇦🇷👆' 'Hola'
+ 'Around' '🫐' 'A' 'Para' 'Desde' 'Gracias' 'An' 'Comparto' 'Leo' 'Empezó'
+ 'To' 'Embajador' '🇦🇷⚽️' 'جماهير' 'Más' 'Estos' 'Atardeceres'
+ 'Repercusiones' '💪🇦🇷' 'Junto' 'With' 'Puerto' 'Como' '🤩' '⏰' '🍻' 'Mural'
+ '👇' 'صحيفة' '@LuccoMarcelo' 'سكالوني' '😍' '45' '¡Felicitaciones' '8'
+ 'It’s' '¡Y' 'Jueves' '#Qatar' '🪪' '¿Vas' '¡FALTA' '🍊🍊' '@gustrivi' '🫐🫐🫐'
+ 'Every' '¿Todavía' '32' '¡Fiesta' 'Located' '974' 'Abu' 'Those'
+ 'Arrangements' 'Qatari' 'Fans' '#Reconocimiento' '¡Si' 'طرح' 'Entre'
+ 'Cerramos' '🇦🇷❄️' 'Proyección' '🇬🇧Two' '🗣' 'Almuerzo' '🐮🍊' 'Is'
+ 'Camiseta' 'Visita' 'Three' '🚨' '11' 'Se' '¡Camiseta' '🗓' '📽' '#Maradona'
+ '🔸' 'Boletín' '"Qatar' 'Y' 'عاجل' 'INVITACION:' 'Brasil' '👆😄👆'
+ '¡Felicitaciones!' '🐦' 'Former' 'Siguen' '¡Momentos' 'خافيير' 'In'
+ 'Tweet' 'Flag' 'Aquí' 'Ceremonia' '¡No' 'One' 'من' 'SOLO.' '⚽️' 'Copa'
+ '🔥🇦🇷🔥' 'Show' 'بابو']</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>['#United2026', '#hiring', '#ProtectJournalist', '#Canadians', '#QNA_Sport', '#ServicesConsulaires', '#Afghanistan', '#QNA_Infographic', '#Scoring4TheGoals', '#cdnag', '#SDG', '#Qatar', '#ItsNotJust', '#Belgique.', '#16DaysOfActivism', '#SDGs', '#HumanRights', '#Canadian', '#Qatar22?', '#FIFAWorldCup', '#16Days.', '#ConsularServices', '#Canadians,', '#FIFA26', '#FIFACoupeduMonde2022', '#UNDay:', '#FIFAWorldCup.', '#youth', '#Qatar!⚽️', '#SDG.', '#ICSC', '#2022FIFAWorldCupQatar', '#WeCAN', '#Belgium.', '#Qatar!', '#FIFACoupeduMonde2022:', '#Qatar_2022', '#Canadiens,', '#Canadien', '#CANMNT', '#CoupeDuMonde', '#QatarGov', '#Canadiens', '#WorldCupQatar2022', '#SDGMoments', '#EmbassyofCanada', '#كأس_العالم_قطر_2022', '#IndoPacific', '#2022FIFAWorldCup', '#Xinjiang.']</t>
+          <t>[nan 'Today' 'Congratulations,' 'Well-done' 'Listen:' 'Proud' 'A' 'Today,'
+ 'In' 'Il' 'Engaging' 'Vous' 'You' 'Un' 'Nous' 'We' 'Honourable'
+ 'Minister' 'Le' 'HOW' 'Morning' '#2022FIFAWorldCup' 'Consiel' '6' 'The'
+ '26' 'Canada' '13' '#QNA_Infographic' 'Media' 'Conseil' '🇨🇦' '20' 'Notre'
+ 'Our' 'Attention!' '30' '27' 'Planning' '#FIFACoupeduMonde2022' '48']</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>['#COP27']</t>
+          <t>[nan 'Day']</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>['#GBV', '#كأس_العالم_قطر_2022،', '#NDEAM.', '#اليوم_العالمي_للإيدز،', '#WorldCupCountdown', '#HumanRights', '#أزمة_المناخ.', '#شهر_التراث_الهسباني', '#UKinQatar', '#Doha.', '#2022.', '#أسبوع_الوقاية_من_الحرائق', '#COP27!', '#IndigenousPeoplesDay', '#SpecialAdvisorDisability', '#YALI2019', '#WAD2022', '#GoUSA2022', '#الأمن_الغذائي', '#WorldCup2022.', '#COP27,', '#TBT', '#16Days', '#CUFFITCHALLENGE', '#SDGMoments', '#SDGs.', '#BreastCancerAwarenessMonth', '#BehindTheScenes', '#US.', '#GenderDay', '#WorldCup', '#HispanicHeritageMonth', '#كأس_العالم_2022', '#WorldCup2022!', '#Election2022', '#يوم_التطوع_العالمي،', '#SportsDiplomacy', '#مع_العنابي_لاخر_مباراة', '#الأطوم', '#WorldMentalHealthDay', '#USWNT', '#2023!', '#FriendshipBench', '#1', '#WorldCup2022', '#كأس_العالم_2026', '#EndHumanTrafficking', '#كأس_العالم2022', '#ExchangeAlumni', '#COP27', '#ExchangeOurWorld', '#MerryChristmas', '#InternationalEducationWeek', '#FIFAWorldCup!', '#Qatar', '#Doha', '#StudyWithUs', '#WorldCupWednesday', '#FIFAWorldCup', '#الاتجار_بالبشر.', '#HappyHolidays', '#DYK', '#WorldAIDSDay2022,', '#ClimateAdaptation.', '#قطر', '#TIP.', '#EndGBV', '#HIV', '#اليوم_الوطني_القطري', '#BCAM', '#خلف_الكواليس', '#ClimateAction', '#IVLP', '#كأس_العالم_قطر2022.', '#الاسبوع_العالمي_لحقوق_الانسان', '#USMNT', '#EnglandvsUSA', '#USQatar50', '#SafirDavisFiDoha', '#InternationalVolunteerDay,', '#حقوق_الإنسان', '#HumanRightsWeek', '#كأس_العالم_قطر2022', '#USAvsWales', '#اليوم_العالمي_للصحة_النفسية', '#2022!', '#QatarNationalDay', '#OPDAT', '#InternationalReligiousFreedomDay,', '#سرطان_الثدي', '#المستشارة_لحقوق_ذوي_الإعاقات', '#dugong', '#FirePreventionWeek', '#AtlasLions.', '#MandelaFellow', '#WorldCup?', '#قطر_الاكوادور', '#ShareAmerica', '#WorldCup2026', '#IEW22']</t>
+          <t>[nan 'يا' '#TBT' 'The' 'Our' 'Today,' 'What' 'نتقدم' 'سيتم' 'إن' 'Human'
+ 'تهانينا' 'Congratulations' 'How' 'Thanks' 'بمناسبة' 'On' 'حزنّا' 'يبدأ'
+ 'U.S.' 'Today' 'نهنئ' 'American' 'سيخوض' 'قال' 'بالتوفيق' 'Good'
+ 'Friday’s' 'Pleased' 'يواجه' 'المباراة' '🇺🇸&amp;amp;🇶🇦' "We're" 'Traveling'
+ 'Celebrate' 'Grateful' 'Exciting' 'With' 'GOOOOAAAL!' 'One' 'Are' 'بعد'
+ 'Si' 'If' "It's" 'Don’t' 'El' 'Qatar’s' 'In' 'It' 'RT' 'America' 'Museum'
+ 'Calling' '#خلف_الكواليس' '#BehindTheScenes' 'أقل' 'Five' 'Hello' 'هذا'
+ 'This' 'يعملون' 'ساعد' 'شهر' 'October' 'Ready' 'We’re' 'Ambassador'
+ 'Mental' 'أقام' 'Last' 'Indigenous' 'من' 'Many' 'Qatar' 'اجتمع' 'Experts'
+ 'متواجدة' 'Working']</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>['#Katar2022', '#FIFAWorldCup2022Qatar', '#StandWithUkraine', '#Hayya.', '#AmicusOeconomiae', '#FerghanaVocationalandTechnicalSchool', '#QatarWorldCup2022', '#RobertLewandowski', '#RememberGusen', '#FIFA2022', '#OTD', '#Qatar', '#RuzziaUnmasked', '#MauthausenMemorial', '#PZPN', '#energy', '#FIFAWorldCup', '#TyzieńSłużbyZagranicznej', '#NobelPeacePrize', '#GeodiversityDay,', '#ForeignServiceWeekPL', '#FIFAWorldCupQatar2022', '#Szczesny💟⚽️', '#FIFAWorldCup2022', '#PolishAid', '#Mauthausen', '#Katar', '#Gusen', '#قطر2022،', '#rememberGusen', '#Polki', '#FergańskaSzkołaZawodowoTechniczna', '#MEXPOL', '#RuZZiaUnmasked', '#NobelPeacePrize.🕊️', '#NobelPrize', '#KierunekKatar', '#SoundInTheSilence2022', '#paszport', '#FIFA']</t>
+          <t>['Today,' nan 'Mikołajki' "Russia's" 'Ales' 'The' '#Szczesny💟⚽️' 'In'
+ '⚠️Paszport' '#RobertLewandowski' 'TO' 'Za' 'Oficjalny' '⏬️W' '⚽️Przed'
+ 'Dzień' '2️⃣2️⃣' 'Wwóz' '⚽️Wybierasz' '⚠️Do' 'This' 'During' 'Z'
+ '⚽️Udostępniliśmy' '⚽️' '💬' '#OTD' '#Polki' 'اللجنة' 'Modern' 'لا'
+ 'Massive' "'When" 'How' "It's" '📺PM' 'On']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added tweet with photo & tweet with image count
</commit_message>
<xml_diff>
--- a/interim/global_embassies_stats.xlsx
+++ b/interim/global_embassies_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -951,7 +951,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>['fr' 'en' 'nl' 'undetected' 'ar']</t>
+          <t>['nl' 'en' 'fr' 'undetected']</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -976,7 +976,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>['en' 'mk' 'ar' 'hr' 'fr' 'tr' 'id']</t>
+          <t>['en' 'mk' 'ar' 'hr' 'sl' 'fr' 'tr' 'id']</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -986,7 +986,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>['en' 'ar' 'undetected' 'so' 'cy']</t>
+          <t>['en' 'ar' 'undetected' 'cy' 'so']</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -1263,6 +1263,128 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>hasImages</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>41</v>
+      </c>
+      <c r="C8" t="n">
+        <v>22</v>
+      </c>
+      <c r="D8" t="n">
+        <v>56</v>
+      </c>
+      <c r="E8" t="n">
+        <v>9</v>
+      </c>
+      <c r="F8" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" t="n">
+        <v>233</v>
+      </c>
+      <c r="H8" t="n">
+        <v>7</v>
+      </c>
+      <c r="I8" t="n">
+        <v>84</v>
+      </c>
+      <c r="J8" t="n">
+        <v>9</v>
+      </c>
+      <c r="K8" t="n">
+        <v>118</v>
+      </c>
+      <c r="L8" t="n">
+        <v>35</v>
+      </c>
+      <c r="M8" t="n">
+        <v>3</v>
+      </c>
+      <c r="N8" t="n">
+        <v>262</v>
+      </c>
+      <c r="O8" t="n">
+        <v>306</v>
+      </c>
+      <c r="P8" t="n">
+        <v>62</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>1</v>
+      </c>
+      <c r="R8" t="n">
+        <v>66</v>
+      </c>
+      <c r="S8" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>hasVideos</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>14</v>
+      </c>
+      <c r="C9" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" t="n">
+        <v>6</v>
+      </c>
+      <c r="E9" t="n">
+        <v>14</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>88</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>43</v>
+      </c>
+      <c r="L9" t="n">
+        <v>14</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>98</v>
+      </c>
+      <c r="O9" t="n">
+        <v>92</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>1</v>
+      </c>
+      <c r="R9" t="n">
+        <v>29</v>
+      </c>
+      <c r="S9" t="n">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>